<commit_message>
completed with sending email
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreeh\OneDrive\Documents\UiPath\ACME-RoboticEnterpriseFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA19A1C-A5A3-48FB-A941-85925A19056E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C921E69-6023-4560-8270-0AF7B95D0E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -171,10 +171,13 @@
     <t>ACME_DownloadFilePath</t>
   </si>
   <si>
+    <t>boolRerun</t>
+  </si>
+  <si>
+    <t>EMAIL_Cred</t>
+  </si>
+  <si>
     <t>sreeharis1999@gmail.com's workspace</t>
-  </si>
-  <si>
-    <t>boolRerun</t>
   </si>
 </sst>
 </file>
@@ -226,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,6 +239,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -613,8 +617,8 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
-        <v>48</v>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -642,13 +646,20 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2813,8 +2824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2869,7 +2880,7 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -2880,7 +2891,7 @@
         <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>